<commit_message>
An exercise tracking app. For now users will type their expense entries on the cli. The app exports and updates an excel file tracking expenses for the user.
</commit_message>
<xml_diff>
--- a/track_temp.xlsx
+++ b/track_temp.xlsx
@@ -398,11 +398,21 @@
           <t>Transportation</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>Retail &amp; Groceries</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>200</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
V1 of the expenses tracking app.
</commit_message>
<xml_diff>
--- a/track_temp.xlsx
+++ b/track_temp.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="270" yWindow="570" windowWidth="20775" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="145621" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -28,6 +27,7 @@
     <font>
       <name val="Times New Roman"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,7 +55,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -350,19 +350,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -398,10 +394,18 @@
           <t>Transportation</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D2" t="n">
+        <v>600</v>
+      </c>
+      <c r="E2">
+        <f>D2-C2</f>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -410,10 +414,18 @@
           <t>Retail &amp; Groceries</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+      <c r="B3" t="n">
+        <v>200</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <f>D3-C3</f>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -422,12 +434,57 @@
           <t>Entertainment</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>300</v>
+      </c>
+      <c r="C4" t="n">
+        <v>350</v>
+      </c>
+      <c r="D4" t="n">
+        <v>450</v>
+      </c>
+      <c r="E4">
+        <f>D4-C4</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Restaurants</t>
         </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>764</v>
+      </c>
+      <c r="D5" t="n">
+        <v>800</v>
+      </c>
+      <c r="E5">
+        <f>D5-C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Total ($)</t>
+        </is>
+      </c>
+      <c r="C6">
+        <f>SUM(C2:C5)</f>
+        <v/>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
+        <v/>
+      </c>
+      <c r="E6">
+        <f>SUM(E2:E5)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>